<commit_message>
added sprint 2 story acceptance criteria
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mhk4cGlUiodmKpozPfkYli0cjJoOg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mggsu2T1CQecvLC21zHhfAyGHpi6w=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Instructions</t>
   </si>
@@ -123,10 +123,22 @@
     <t>As a Player I want to move my checkers diagonally forward so that I can advance my checkers.</t>
   </si>
   <si>
+    <t>Given it is my turn when I select a square to move to then my piece moves to that square.</t>
+  </si>
+  <si>
     <t>As a Player I want to be able to jump over an opponent player’s piece so that I can take that piece.</t>
   </si>
   <si>
+    <t>Given it is my turn when select a space diagonally behind my opponent then to take my opponent's piece.</t>
+  </si>
+  <si>
+    <t>Given there is a capture available for me when I make a move then the move has to be a capture.</t>
+  </si>
+  <si>
     <t>As a Player I want to be able to jump over multiple opponent pieces so that I can take multiple pieces in one turn.</t>
+  </si>
+  <si>
+    <t>Given there are multiple jump moves available when make a jump move then my turn resets allowing me to make another jump move.</t>
   </si>
   <si>
     <t>As a Player I want to resign the game I am playing so that I am done playing.</t>
@@ -159,7 +171,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -177,12 +188,13 @@
     </font>
     <font>
       <sz val="12.0"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
     </font>
+    <font/>
     <font>
       <sz val="12.0"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-Calibri"/>
+      <color theme="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -215,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -229,23 +241,23 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -254,29 +266,32 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4179,9 +4194,11 @@
       <c r="A19" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="21"/>
+      <c r="B19" s="20" t="s">
+        <v>33</v>
+      </c>
       <c r="C19" s="11"/>
-      <c r="D19" s="22"/>
+      <c r="D19" s="2"/>
       <c r="E19" s="11"/>
       <c r="F19" s="2"/>
       <c r="G19" s="11"/>
@@ -4206,10 +4223,12 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="20" t="s">
-        <v>33</v>
+      <c r="A20" s="21" t="s">
+        <v>34</v>
       </c>
-      <c r="B20" s="21"/>
+      <c r="B20" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="C20" s="11"/>
       <c r="D20" s="2"/>
       <c r="E20" s="11"/>
@@ -4236,10 +4255,10 @@
       <c r="Z20" s="12"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="20" t="s">
-        <v>34</v>
+      <c r="A21" s="22"/>
+      <c r="B21" s="20" t="s">
+        <v>36</v>
       </c>
-      <c r="B21" s="21"/>
       <c r="C21" s="11"/>
       <c r="D21" s="2"/>
       <c r="E21" s="11"/>
@@ -4266,10 +4285,12 @@
       <c r="Z21" s="12"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="20" t="s">
-        <v>35</v>
+      <c r="A22" s="22" t="s">
+        <v>37</v>
       </c>
-      <c r="B22" s="21"/>
+      <c r="B22" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="C22" s="11"/>
       <c r="D22" s="2"/>
       <c r="E22" s="11"/>
@@ -4296,10 +4317,10 @@
       <c r="Z22" s="12"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="20" t="s">
-        <v>36</v>
+      <c r="A23" s="22" t="s">
+        <v>39</v>
       </c>
-      <c r="B23" s="21"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="11"/>
       <c r="D23" s="2"/>
       <c r="E23" s="11"/>
@@ -4326,10 +4347,10 @@
       <c r="Z23" s="12"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="20" t="s">
-        <v>37</v>
+      <c r="A24" s="22" t="s">
+        <v>40</v>
       </c>
-      <c r="B24" s="21"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="11"/>
       <c r="D24" s="2"/>
       <c r="E24" s="11"/>
@@ -4356,8 +4377,10 @@
       <c r="Z24" s="12"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="A25" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="23"/>
       <c r="C25" s="11"/>
       <c r="D25" s="2"/>
       <c r="E25" s="11"/>
@@ -9846,11 +9869,11 @@
     <row r="221" ht="15.75" customHeight="1">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
-      <c r="C221" s="2"/>
+      <c r="C221" s="11"/>
       <c r="D221" s="2"/>
-      <c r="E221" s="2"/>
+      <c r="E221" s="11"/>
       <c r="F221" s="2"/>
-      <c r="G221" s="2"/>
+      <c r="G221" s="11"/>
       <c r="H221" s="2"/>
       <c r="I221" s="12"/>
       <c r="J221" s="12"/>
@@ -31683,38 +31706,66 @@
       <c r="Y1000" s="12"/>
       <c r="Z1000" s="12"/>
     </row>
+    <row r="1001" ht="15.75" customHeight="1">
+      <c r="A1001" s="2"/>
+      <c r="B1001" s="2"/>
+      <c r="C1001" s="2"/>
+      <c r="D1001" s="2"/>
+      <c r="E1001" s="2"/>
+      <c r="F1001" s="2"/>
+      <c r="G1001" s="2"/>
+      <c r="H1001" s="2"/>
+      <c r="I1001" s="12"/>
+      <c r="J1001" s="12"/>
+      <c r="K1001" s="12"/>
+      <c r="L1001" s="12"/>
+      <c r="M1001" s="12"/>
+      <c r="N1001" s="12"/>
+      <c r="O1001" s="12"/>
+      <c r="P1001" s="12"/>
+      <c r="Q1001" s="12"/>
+      <c r="R1001" s="12"/>
+      <c r="S1001" s="12"/>
+      <c r="T1001" s="12"/>
+      <c r="U1001" s="12"/>
+      <c r="V1001" s="12"/>
+      <c r="W1001" s="12"/>
+      <c r="X1001" s="12"/>
+      <c r="Y1001" s="12"/>
+      <c r="Z1001" s="12"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
     <mergeCell ref="G17:G18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="D17:D18"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:C1000 E2:E1000 G2:G1000">
+  <conditionalFormatting sqref="C2:C1001 E2:E1001 G2:G1001">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C1000 E2:E1000 G2:G1000">
+  <conditionalFormatting sqref="C2:C1001 E2:E1001 G2:G1001">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D1000 F2:F1000 H2:H1000">
+  <conditionalFormatting sqref="D2:D1001 F2:F1001 H2:H1001">
     <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D1000 F2:F1000 H2:H1000">
+  <conditionalFormatting sqref="D2:D1001 F2:F1001 H2:H1001">
     <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C17 E2:E17 G2:G17 C19:C597 E19:E597 G19:G597">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C17 E2:E17 G2:G17 C19:C598 E19:E598 G19:G598">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added unit tests + updated ac
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mggsu2T1CQecvLC21zHhfAyGHpi6w=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mhJF6uD7JMLjpiFC8od5CPZOox8FA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>Instructions</t>
   </si>
@@ -132,13 +132,22 @@
     <t>Given it is my turn when I select a square to move to then my piece moves to that square.</t>
   </si>
   <si>
+    <t>ZE 10/21</t>
+  </si>
+  <si>
+    <t>Given it is my turn when I select a square that has another piece on it then I cannot move to that square.</t>
+  </si>
+  <si>
+    <t>Given it is not my turn when my opponent makes a move then it should be shown on the board.</t>
+  </si>
+  <si>
     <t>As a Player I want to be able to jump over an opponent player’s piece so that I can take that piece.</t>
   </si>
   <si>
     <t>Given it is my turn when select a space diagonally behind my opponent then to take my opponent's piece.</t>
   </si>
   <si>
-    <t>Given there is a capture available for me when I make a move then the move has to be a capture.</t>
+    <t>Given there is a capture available for me whenI make a move then the move removes the opponent piece.</t>
   </si>
   <si>
     <t>As a Player I want to be able to jump over multiple opponent pieces so that I can take multiple pieces in one turn.</t>
@@ -160,7 +169,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -197,10 +206,6 @@
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
     </font>
-    <font>
-      <sz val="12.0"/>
-      <color theme="1"/>
-    </font>
     <font/>
   </fonts>
   <fills count="3">
@@ -233,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -287,13 +292,10 @@
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -3981,7 +3983,7 @@
       <c r="E11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="10" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="11"/>
@@ -4176,7 +4178,7 @@
       <c r="Z16" s="12"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="19" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="16"/>
@@ -4206,8 +4208,8 @@
       <c r="Z17" s="12"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
       <c r="H18" s="2"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -4229,16 +4231,20 @@
       <c r="Z18" s="12"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="2"/>
+      <c r="E19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="G19" s="11"/>
       <c r="H19" s="2"/>
       <c r="I19" s="12"/>
@@ -4261,16 +4267,18 @@
       <c r="Z19" s="12"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="10" t="s">
-        <v>36</v>
-      </c>
+      <c r="A20" s="10"/>
       <c r="B20" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>36</v>
+      </c>
       <c r="G20" s="11"/>
       <c r="H20" s="2"/>
       <c r="I20" s="12"/>
@@ -4293,14 +4301,18 @@
       <c r="Z20" s="12"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22" t="s">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="2"/>
+      <c r="E21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>36</v>
+      </c>
       <c r="G21" s="11"/>
       <c r="H21" s="2"/>
       <c r="I21" s="12"/>
@@ -4323,16 +4335,20 @@
       <c r="Z21" s="12"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="2"/>
+      <c r="E22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="G22" s="11"/>
       <c r="H22" s="2"/>
       <c r="I22" s="12"/>
@@ -4355,14 +4371,18 @@
       <c r="Z22" s="12"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="23"/>
       <c r="C23" s="11"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="2"/>
+      <c r="E23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="G23" s="11"/>
       <c r="H23" s="2"/>
       <c r="I23" s="12"/>
@@ -4385,10 +4405,12 @@
       <c r="Z23" s="12"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="23"/>
+      <c r="B24" s="21" t="s">
+        <v>43</v>
+      </c>
       <c r="C24" s="11"/>
       <c r="D24" s="2"/>
       <c r="E24" s="11"/>
@@ -4415,10 +4437,10 @@
       <c r="Z24" s="12"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="22" t="s">
-        <v>43</v>
+      <c r="A25" s="21" t="s">
+        <v>44</v>
       </c>
-      <c r="B25" s="23"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="11"/>
       <c r="D25" s="2"/>
       <c r="E25" s="11"/>
@@ -4445,8 +4467,10 @@
       <c r="Z25" s="12"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+      <c r="A26" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="22"/>
       <c r="C26" s="11"/>
       <c r="D26" s="2"/>
       <c r="E26" s="11"/>
@@ -4473,8 +4497,10 @@
       <c r="Z26" s="12"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="22"/>
       <c r="C27" s="11"/>
       <c r="D27" s="2"/>
       <c r="E27" s="11"/>
@@ -9935,11 +9961,11 @@
     <row r="222" ht="15.75" customHeight="1">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
-      <c r="C222" s="2"/>
+      <c r="C222" s="11"/>
       <c r="D222" s="2"/>
-      <c r="E222" s="2"/>
+      <c r="E222" s="11"/>
       <c r="F222" s="2"/>
-      <c r="G222" s="2"/>
+      <c r="G222" s="11"/>
       <c r="H222" s="2"/>
       <c r="I222" s="12"/>
       <c r="J222" s="12"/>
@@ -9963,11 +9989,11 @@
     <row r="223" ht="15.75" customHeight="1">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
-      <c r="C223" s="2"/>
+      <c r="C223" s="11"/>
       <c r="D223" s="2"/>
-      <c r="E223" s="2"/>
+      <c r="E223" s="11"/>
       <c r="F223" s="2"/>
-      <c r="G223" s="2"/>
+      <c r="G223" s="11"/>
       <c r="H223" s="2"/>
       <c r="I223" s="12"/>
       <c r="J223" s="12"/>
@@ -31772,6 +31798,62 @@
       <c r="Y1001" s="12"/>
       <c r="Z1001" s="12"/>
     </row>
+    <row r="1002" ht="15.75" customHeight="1">
+      <c r="A1002" s="2"/>
+      <c r="B1002" s="2"/>
+      <c r="C1002" s="2"/>
+      <c r="D1002" s="2"/>
+      <c r="E1002" s="2"/>
+      <c r="F1002" s="2"/>
+      <c r="G1002" s="2"/>
+      <c r="H1002" s="2"/>
+      <c r="I1002" s="12"/>
+      <c r="J1002" s="12"/>
+      <c r="K1002" s="12"/>
+      <c r="L1002" s="12"/>
+      <c r="M1002" s="12"/>
+      <c r="N1002" s="12"/>
+      <c r="O1002" s="12"/>
+      <c r="P1002" s="12"/>
+      <c r="Q1002" s="12"/>
+      <c r="R1002" s="12"/>
+      <c r="S1002" s="12"/>
+      <c r="T1002" s="12"/>
+      <c r="U1002" s="12"/>
+      <c r="V1002" s="12"/>
+      <c r="W1002" s="12"/>
+      <c r="X1002" s="12"/>
+      <c r="Y1002" s="12"/>
+      <c r="Z1002" s="12"/>
+    </row>
+    <row r="1003" ht="15.75" customHeight="1">
+      <c r="A1003" s="2"/>
+      <c r="B1003" s="2"/>
+      <c r="C1003" s="2"/>
+      <c r="D1003" s="2"/>
+      <c r="E1003" s="2"/>
+      <c r="F1003" s="2"/>
+      <c r="G1003" s="2"/>
+      <c r="H1003" s="2"/>
+      <c r="I1003" s="12"/>
+      <c r="J1003" s="12"/>
+      <c r="K1003" s="12"/>
+      <c r="L1003" s="12"/>
+      <c r="M1003" s="12"/>
+      <c r="N1003" s="12"/>
+      <c r="O1003" s="12"/>
+      <c r="P1003" s="12"/>
+      <c r="Q1003" s="12"/>
+      <c r="R1003" s="12"/>
+      <c r="S1003" s="12"/>
+      <c r="T1003" s="12"/>
+      <c r="U1003" s="12"/>
+      <c r="V1003" s="12"/>
+      <c r="W1003" s="12"/>
+      <c r="X1003" s="12"/>
+      <c r="Y1003" s="12"/>
+      <c r="Z1003" s="12"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A17:A18"/>
@@ -31782,28 +31864,28 @@
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="G17:G18"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:C1001 E2:E1001 G2:G1001">
+  <conditionalFormatting sqref="C2:C1003 E2:E1003 G2:G1003">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C1001 E2:E1001 G2:G1001">
+  <conditionalFormatting sqref="C2:C1003 E2:E1003 G2:G1003">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D1001 F2:F1001 H2:H1001">
+  <conditionalFormatting sqref="D2:D1003 F2:F1003 H2:H1003">
     <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D1001 F2:F1001 H2:H1001">
+  <conditionalFormatting sqref="D2:D1003 F2:F1003 H2:H1003">
     <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C17 E2:E17 G2:G17 C19:C598 E19:E598 G19:G598">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C17 E2:E17 G2:G17 C19:C600 E19:E600 G19:G600">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>